<commit_message>
sync for customer hearing on 9/06 2019.
</commit_message>
<xml_diff>
--- a/_project_docs/SSE19_RD_CD.xlsx
+++ b/_project_docs/SSE19_RD_CD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\workplace\smartse19\_project_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FE9646-7B94-4A13-B6C6-18E461D97761}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0784B39-E7E2-4BE4-9C86-38413279BAF8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4050" yWindow="1350" windowWidth="20820" windowHeight="11835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28005" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Code Design" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="168">
   <si>
     <t>No</t>
   </si>
@@ -216,9 +216,6 @@
     <t>就寝</t>
   </si>
   <si>
-    <t>仕事</t>
-  </si>
-  <si>
     <t>歩行</t>
   </si>
   <si>
@@ -535,6 +532,18 @@
   </si>
   <si>
     <t>app category</t>
+  </si>
+  <si>
+    <t>仕事(office)</t>
+  </si>
+  <si>
+    <t>仕事(home)</t>
+  </si>
+  <si>
+    <t>会議</t>
+  </si>
+  <si>
+    <t>meeting</t>
   </si>
 </sst>
 </file>
@@ -4513,10 +4522,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4563,7 +4572,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -4577,15 +4586,15 @@
         <v>2</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G6" s="7"/>
     </row>
@@ -4595,15 +4604,15 @@
         <v>3</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>69</v>
       </c>
       <c r="G7" s="7"/>
     </row>
@@ -4613,15 +4622,15 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>71</v>
       </c>
       <c r="G8" s="7"/>
     </row>
@@ -4631,15 +4640,15 @@
         <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="G9" s="7"/>
     </row>
@@ -4649,25 +4658,25 @@
         <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>75</v>
       </c>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <f t="shared" ref="A11:A35" si="1">ROW()-4</f>
+        <f t="shared" ref="A11:A38" si="1">ROW()-4</f>
         <v>7</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -4681,7 +4690,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>16</v>
@@ -4701,7 +4710,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>16</v>
@@ -4738,14 +4747,16 @@
         <v>48</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="7"/>
+        <v>84</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>76</v>
+      </c>
       <c r="E15" s="7" t="s">
         <v>47</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>58</v>
+        <v>164</v>
       </c>
       <c r="G15" s="7"/>
     </row>
@@ -4758,18 +4769,20 @@
         <v>48</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7" t="s">
-        <v>21</v>
+        <v>84</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>57</v>
+        <v>166</v>
       </c>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -4778,38 +4791,42 @@
         <v>48</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7" t="s">
-        <v>7</v>
+        <v>84</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
-        <f t="shared" si="1"/>
+        <f>ROW()-4</f>
         <v>14</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="7"/>
+        <v>84</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="E18" s="7" t="s">
-        <v>108</v>
+        <v>47</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>109</v>
+        <v>165</v>
       </c>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -4818,18 +4835,20 @@
         <v>48</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="7"/>
+        <v>84</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="E19" s="4" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -4838,20 +4857,20 @@
         <v>48</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="4" t="s">
-        <v>22</v>
+        <v>84</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -4860,18 +4879,18 @@
         <v>48</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D21" s="7"/>
-      <c r="E21" s="4" t="s">
-        <v>49</v>
+      <c r="E21" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -4880,18 +4899,18 @@
         <v>48</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D22" s="7"/>
-      <c r="E22" s="4" t="s">
-        <v>56</v>
+      <c r="E22" s="7" t="s">
+        <v>107</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G22" s="7"/>
     </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -4900,20 +4919,18 @@
         <v>48</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D23" s="7"/>
-      <c r="E23" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -4922,16 +4939,18 @@
         <v>48</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D24" s="7"/>
-      <c r="E24" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="G24" s="13"/>
+      <c r="E24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
@@ -4942,20 +4961,18 @@
         <v>48</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D25" s="7"/>
-      <c r="E25" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -4964,18 +4981,20 @@
         <v>48</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D26" s="7"/>
-      <c r="E26" s="15" t="s">
-        <v>24</v>
+      <c r="E26" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" s="13"/>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -4984,20 +5003,18 @@
         <v>48</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="15" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="G27" s="13"/>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -5006,17 +5023,17 @@
         <v>48</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D28" s="7"/>
-      <c r="E28" s="16" t="s">
-        <v>26</v>
+      <c r="E28" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -5028,51 +5045,79 @@
         <v>48</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D29" s="7"/>
-      <c r="E29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="13"/>
+    </row>
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
+      <c r="B30" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E30" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+      <c r="B31" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
+      <c r="E31" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
+      <c r="B32" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="E32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -5112,31 +5157,40 @@
       <c r="G35" s="7"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
+      <c r="A36" s="6">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
+      <c r="A37" s="6">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
+      <c r="A38" s="6">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
@@ -5148,13 +5202,40 @@
       <c r="G39" s="6"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:G4" xr:uid="{59021625-C2CE-4FC9-910D-D045D7CD2E5F}"/>
@@ -5219,13 +5300,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -5237,19 +5318,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G6" s="7"/>
     </row>
@@ -5259,19 +5340,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G7" s="7"/>
     </row>
@@ -5281,19 +5362,19 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G8" s="7"/>
     </row>
@@ -5303,19 +5384,19 @@
         <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G9" s="7"/>
     </row>
@@ -5325,19 +5406,19 @@
         <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E10" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>105</v>
       </c>
       <c r="G10" s="7"/>
     </row>
@@ -5347,19 +5428,19 @@
         <v>7</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E11" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>106</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>107</v>
       </c>
       <c r="G11" s="7"/>
     </row>
@@ -5369,10 +5450,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -5385,10 +5466,10 @@
         <v>9</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>41</v>
@@ -5407,10 +5488,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>41</v>
@@ -5429,10 +5510,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>42</v>
@@ -5441,7 +5522,7 @@
         <v>45</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G15" s="7"/>
     </row>
@@ -5451,10 +5532,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>42</v>
@@ -5466,7 +5547,7 @@
         <v>20</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -5475,10 +5556,10 @@
         <v>13</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -5491,10 +5572,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7" t="s">
@@ -5511,20 +5592,20 @@
         <v>15</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -5533,10 +5614,10 @@
         <v>16</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7" t="s">
@@ -5553,7 +5634,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>21</v>
@@ -5569,17 +5650,17 @@
         <v>18</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G22" s="7"/>
     </row>
@@ -5589,17 +5670,17 @@
         <v>19</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G23" s="7"/>
     </row>
@@ -5609,17 +5690,17 @@
         <v>20</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G24" s="7"/>
     </row>
@@ -5629,10 +5710,10 @@
         <v>21</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -5645,19 +5726,19 @@
         <v>22</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>114</v>
-      </c>
       <c r="E26" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G26" s="7"/>
     </row>
@@ -5667,19 +5748,19 @@
         <v>23</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>115</v>
-      </c>
       <c r="F27" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G27" s="7"/>
     </row>
@@ -5689,19 +5770,19 @@
         <v>24</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>114</v>
-      </c>
       <c r="E28" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G28" s="7"/>
     </row>
@@ -5711,7 +5792,7 @@
         <v>25</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -5725,7 +5806,7 @@
         <v>26</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>15</v>
@@ -5745,7 +5826,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>15</v>
@@ -5758,7 +5839,7 @@
         <v>37</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5767,7 +5848,7 @@
         <v>28</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>15</v>
@@ -5780,7 +5861,7 @@
         <v>40</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -5789,7 +5870,7 @@
         <v>29</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>15</v>
@@ -5802,7 +5883,7 @@
         <v>39</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5811,20 +5892,20 @@
         <v>30</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F34" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="G34" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -5957,7 +6038,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6004,7 +6085,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -6018,14 +6099,14 @@
         <v>2</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -6036,14 +6117,14 @@
         <v>3</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -6054,14 +6135,14 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -6072,14 +6153,14 @@
         <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -6090,14 +6171,14 @@
         <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -6108,14 +6189,14 @@
         <v>7</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="7"/>
@@ -6126,14 +6207,14 @@
         <v>8</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -6144,14 +6225,14 @@
         <v>9</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -6162,14 +6243,14 @@
         <v>10</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -6180,14 +6261,14 @@
         <v>11</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -6198,14 +6279,14 @@
         <v>12</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -6216,14 +6297,14 @@
         <v>13</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
@@ -6234,14 +6315,14 @@
         <v>14</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -6252,14 +6333,14 @@
         <v>15</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -6270,14 +6351,14 @@
         <v>16</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
@@ -6288,14 +6369,14 @@
         <v>17</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -6306,14 +6387,14 @@
         <v>18</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -6324,14 +6405,14 @@
         <v>19</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -6342,14 +6423,14 @@
         <v>20</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
@@ -6360,14 +6441,14 @@
         <v>21</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -6378,14 +6459,14 @@
         <v>22</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
@@ -6396,14 +6477,14 @@
         <v>23</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
@@ -6414,14 +6495,14 @@
         <v>24</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
@@ -6432,14 +6513,14 @@
         <v>25</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
@@ -6450,14 +6531,14 @@
         <v>26</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
@@ -6468,14 +6549,14 @@
         <v>27</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>

</xml_diff>